<commit_message>
updating lecture demo for tomorrow
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -464,7 +464,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[Structural balance demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flecture%2F20240919_structural_balance%2Fstructural_balance_in_the_small_slashdot_network.ipynb)</t>
+          <t>[Structural balance demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flecture%2F20250908_structural_balance%2Fstructural_balance_in_the_small_slashdot_network.ipynb)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -501,16 +501,16 @@
           <t>[Lab 3: Enriching network data and testing a hypothesis about homophily](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab03%2Flab03_homophily.ipynb)</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Mini Project 02: Complete network data</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="D8" t="inlineStr">
         <is>
           <t>Network centrality / the Friendship Paradox</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Mini Project 02: Complete network data</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added lab 3, hopefully
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -491,14 +491,9 @@
           <t>Networks in context; homophily; affiliation networks; and foci</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>[Two mode network demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flecture%2F20240917_two_mode_networks%2Ftwo_mode_networks.ipynb)</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[Lab 3: Enriching network data and testing a hypothesis about homophily](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab03%2Flab03_homophily.ipynb)</t>
+          <t>[Lab 3: Enriching network data and testing a hypothesis about homophily](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flab%2Flab03%2Flab03_homophily.ipynb)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update syllabus + lecture demos
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -527,7 +527,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[Lab 4 - Two-mode networks](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab05%2Flab05_two_mode_networks.ipynb)</t>
+          <t>[Lab 4 - ER Model](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2025%2Flab%2Flab04%2Flab4_clustering_coefficient_er.ipynb)</t>
         </is>
       </c>
     </row>
@@ -549,11 +549,6 @@
           <t>[Lab 5- Exploring the ER model](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab04%2Flab4_clustering_coefficient_er.ipynb)</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>? Problem Set 01</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
@@ -566,6 +561,11 @@
           <t>[netlogo BA model](https://www.netlogoweb.org/launch#https://www.netlogoweb.org/assets/modelslib/Sample%20Models/Networks/Preferential%20Attachment.nlogo)</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>? Problem Set 01</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Empirical studies of network structure</t>
+          <t>More models: configuration model and stochastic block model</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="14">
       <c r="D14" t="inlineStr">
         <is>
-          <t>Midterm review</t>
+          <t>Community detection</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -600,26 +600,26 @@
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>Midterm</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>[Lab 6: Community detection](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab06%2Flab06_community_detection.ipynb)</t>
+          <t>Midterm review</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="D16" t="inlineStr">
         <is>
-          <t>More models: configuration model and stochastic block model</t>
+          <t>Midterm</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>Community detection</t>
+          <t>Empirical studies of network structure</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[Lab 6: Community detection](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab06%2Flab06_community_detection.ipynb)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">

</xml_diff>

<commit_message>
add nov 11 holiday + mini proj 3
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -622,11 +622,6 @@
           <t>[Lab 6 - Community Detection](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flab%2Flab06%2Flab06_community_detection.ipynb)</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>? Mini Project 03</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
@@ -657,11 +652,6 @@
           <t>[Lab 7: Mini Project 3 Prep](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2025%2Flab%2Flab07%2Flab07_mp3_prep.ipynb)</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>? Problem Set 02</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
@@ -674,6 +664,11 @@
           <t>[Network SIR demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Falisonswu%2Fshiny-SimNetwork&amp;urlpath=shiny%2Fshiny-SimNetwork%2F); [Threshold infectiousness demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flecture%2F20251030_sir_threshold_infectiousness%2Fsir_threshold_infectiousness.ipynb)</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>[Mini Project 03: Tudor network](https://docs.google.com/document/d/1XxtW5ZlPzRwHcbTHapKzeSZySq0axOVMnOGFtAnprEY/edit?usp=sharing)</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -710,40 +705,40 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>NO CLASS (HOLIDAY)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>[Social influence](#sec:socialinfluence)</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Social influence, herding, and cascades</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="D24" t="inlineStr">
+    <row r="25">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Threshold models and complex contagion</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>[Dynamics: Complex contagion and social influence](#sec:complexcontagion)</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Complex contagion on networks</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Complex contagion on networks, cont. + Empirical studies of complex contagion</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -767,21 +762,21 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Complex contagion on networks, cont. + Empirical studies of complex contagion</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>[Cooperation](#sec:cooperation)</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Cooperation and networks</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>Wrap up</t>
+          <t>Cooperation and networks / Wrap Up</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Links to concurrency demo + lab 8
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -683,12 +683,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[Concurrency demo](https://shiny.demog.berkeley.edu/dennis/concurrency/)</t>
+          <t>[Concurrency demo](https://datahub.berkeley.edu/user/feehan/shiny/shiny-id-demos/concurrency/)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[Lab 8: Mini-project prep](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2024&amp;branch=main&amp;urlpath=tree%2Fdemog180-fa2024%2Flabs%2Flab08%2Flab08_project_prep.ipynb)</t>
+          <t>[Lab 8: Simple contagion and centrality](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flab%2Flab08%2Flab08_simple_contagion.ipynb)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
switch order (holiday coming up)
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -693,18 +693,28 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>[Social influence](#sec:socialinfluence)</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>Social influence, herding, and cascades</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>? Mini Project 04</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
           <t>Empirical studies of simple contagion</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>? Mini Project 04</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
       <c r="D23" t="inlineStr">
         <is>
           <t>NO CLASS (HOLIDAY)</t>
@@ -712,33 +722,28 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>[Social influence](#sec:socialinfluence)</t>
-        </is>
-      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Social influence, herding, and cascades</t>
+          <t>Threshold models and complex contagion</t>
         </is>
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>[Dynamics: Complex contagion and social influence](#sec:complexcontagion)</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Threshold models and complex contagion</t>
+          <t>Complex contagion on networks</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>[Dynamics: Complex contagion and social influence](#sec:complexcontagion)</t>
-        </is>
-      </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Complex contagion on networks</t>
+          <t>Complex contagion on networks, cont.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -762,21 +767,21 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>[Cooperation](#sec:cooperation)</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Complex contagion on networks, cont. + Empirical studies of complex contagion</t>
+          <t>Cooperation and networks</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>[Cooperation](#sec:cooperation)</t>
-        </is>
-      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Cooperation and networks / Wrap Up</t>
+          <t>Empirical studies / Wrap up</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
rebalancing the next few lectures
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -719,7 +719,7 @@
     <row r="24">
       <c r="D24" t="inlineStr">
         <is>
-          <t>Cascades cont.; Conditional Probability and Bayes's Rule; Threshold models</t>
+          <t>Cascades cont.; Conditional Probability and Bayes's Rule</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -736,14 +736,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Complex contagion on networks</t>
+          <t>Threshold models and complex contagion</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="inlineStr">
         <is>
-          <t>Complex contagion on networks, cont.</t>
+          <t>Complex contagion cont...</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">

</xml_diff>

<commit_message>
add link to axelrod demo
</commit_message>
<xml_diff>
--- a/demog180-syllabus/demog180.xlsx
+++ b/demog180-syllabus/demog180.xlsx
@@ -741,9 +741,19 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>[Cooperation](#sec:cooperation)</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Cooperation and networks</t>
+          <t>Cooperation</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[Axelrod tournament demo](https://datahub.berkeley.edu/hub/user-redirect/git-pull?repo=https%3A%2F%2Fgithub.com%2Fdfeehan%2Fdemog180-fa2025&amp;branch=main&amp;urlpath=lab%2Ftree%2Fdemog180-fa2025%2Flecture%2F20251119_cooperation%2Fipd_tournament.ipynb)</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -772,11 +782,6 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>[Cooperation](#sec:cooperation)</t>
-        </is>
-      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Empirical studies</t>

</xml_diff>